<commit_message>
New version of main
Created new version of main to work on rolling input data, moved old version to Obsolete. Minor changes to other files.
</commit_message>
<xml_diff>
--- a/Workbook.xlsx
+++ b/Workbook.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1034C579-3D13-478C-9E17-0834FBBF1A93}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{128EEE34-7C03-485D-ABDD-BAA63E5ED666}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="33">
   <si>
     <t>Date</t>
   </si>
@@ -31,13 +31,94 @@
     <t>Bugfixing, using full retweeted text (which is the only way to avoid truncated text) cuts off the '@' which stops retweets being used in the network. Have now manually concatinating the frist mention (in a retweet first mention is always the trageted user) back onto each text object</t>
   </si>
   <si>
-    <t>Writing, Looking at previous dissertations and planning the structure of mine</t>
-  </si>
-  <si>
     <t>First day</t>
   </si>
   <si>
     <t>AL</t>
+  </si>
+  <si>
+    <t>Made valid user generator robust to dissconnection and changed it to output a dictonary of ID:screen_name so that in future fast searches can be performed on the ID which is faster to get. Added time feature to topic modeller so you can ask for tweets from X days ago only. Started building sentiment checker.py which will scan for mentions of a user (with the option of adding a topic) and will return the sentiment score of those tweets</t>
+  </si>
+  <si>
+    <t>Fixing disconnection bug in Verified_users_generator, building sentiment checker.py</t>
+  </si>
+  <si>
+    <t>Revewing literature</t>
+  </si>
+  <si>
+    <t>Onboarding, setting up accounts, etc</t>
+  </si>
+  <si>
+    <t>Computer locked out, worked from uni on collecting lit</t>
+  </si>
+  <si>
+    <t>Setting up writing document</t>
+  </si>
+  <si>
+    <t>Started working on core functionality, program takes in a list of authors and tweets, uses the author and @s to build and edge list, feeds the edgelist into the networkx package, generates netwrok statsitics for each user in the network and then reports the top 10</t>
+  </si>
+  <si>
+    <t>Work on core program</t>
+  </si>
+  <si>
+    <t>Implimented hashing function to hide all accounts other than the valid user</t>
+  </si>
+  <si>
+    <t>Work on core program, wrapped in twitter bot for demonstration</t>
+  </si>
+  <si>
+    <t>Feedback on core program that they are intrested in an input user rather than top 10, and also that they can't show nonvalidated users in the results, not intrested in the twitter bot functionality</t>
+  </si>
+  <si>
+    <t>Reworked main program to authenticate from Twitter to get more data</t>
+  </si>
+  <si>
+    <t>Worked on setting up write up doctument</t>
+  </si>
+  <si>
+    <t>Work on literature</t>
+  </si>
+  <si>
+    <t>Investigated methods for identifying valid users</t>
+  </si>
+  <si>
+    <t>Implmented basic method for getting valid users from tweet objects, can get senders, but not recivers</t>
+  </si>
+  <si>
+    <t>Implimented getting recivers valid status by making extra API calls</t>
+  </si>
+  <si>
+    <t>Recivers can be identified as valid if the tweet is a retweet - added that functionality and now only have to make 20% of API calls otherwise would</t>
+  </si>
+  <si>
+    <t>Pivoted main program so it displayed the given user in a distribution of valid users based on percentile rank within the network metrics</t>
+  </si>
+  <si>
+    <t>Changed mian to use full text by using the extended option in tweepy - but retweet text is in a different place from normal mentions so added if statmenets</t>
+  </si>
+  <si>
+    <t>Work on core program, added basic graphing</t>
+  </si>
+  <si>
+    <t>Research on better graphing tools</t>
+  </si>
+  <si>
+    <t>Added a better graphing tool which is written in R, python saves data and then calls an R script which takes the data and saves an HTML graph, finally python opens the HTML to show the graph</t>
+  </si>
+  <si>
+    <t>Built topic modeller script - this takes a given user, scans their sent tweets and returns their most used hashtags and topcis, based on  topic modelling</t>
+  </si>
+  <si>
+    <t>Added sentiment analyis to main - it can now report the sentiment of the whole network as well as tweets about the given user</t>
+  </si>
+  <si>
+    <t>Writing, Looking at previous dissertations and planning the structure of mine, added cheating so tweets send by or about the given user can be added to the network artificially (increases bias)</t>
+  </si>
+  <si>
+    <t>Adapted hasing so valid users and the given user is shown, built verified user generator which will create a JSON of all verified users so no API calls need to be made by the other scripts</t>
+  </si>
+  <si>
+    <t>Work on verified user generator - will take almost 4 days to run, but should only need run once</t>
   </si>
 </sst>
 </file>
@@ -356,10 +437,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B35"/>
+  <dimension ref="A1:B74"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -380,184 +461,466 @@
         <v>43605</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>43606</v>
       </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>43607</v>
       </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>43608</v>
       </c>
+      <c r="B5" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>43609</v>
       </c>
+      <c r="B6" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>43612</v>
       </c>
+      <c r="B7" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>43613</v>
       </c>
+      <c r="B8" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>43614</v>
       </c>
+      <c r="B9" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>43615</v>
       </c>
+      <c r="B10" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>43616</v>
       </c>
+      <c r="B11" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>43619</v>
       </c>
+      <c r="B12" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>43620</v>
       </c>
+      <c r="B13" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>43621</v>
       </c>
+      <c r="B14" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>43622</v>
       </c>
+      <c r="B15" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>43623</v>
       </c>
+      <c r="B16" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
-        <v>43624</v>
+        <v>43626</v>
+      </c>
+      <c r="B17" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
-        <v>43625</v>
+        <v>43627</v>
+      </c>
+      <c r="B18" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
-        <v>43626</v>
+        <v>43628</v>
+      </c>
+      <c r="B19" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
-        <v>43627</v>
+        <v>43629</v>
+      </c>
+      <c r="B20" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
-        <v>43628</v>
+        <v>43630</v>
+      </c>
+      <c r="B21" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
-        <v>43629</v>
+        <v>43633</v>
+      </c>
+      <c r="B22" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
-        <v>43630</v>
+        <v>43634</v>
+      </c>
+      <c r="B23" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
-        <v>43633</v>
+        <v>43635</v>
+      </c>
+      <c r="B24" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
-        <v>43634</v>
+        <v>43636</v>
+      </c>
+      <c r="B25" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
-        <v>43635</v>
+        <v>43637</v>
       </c>
       <c r="B26" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
-        <v>43636</v>
+        <v>43640</v>
+      </c>
+      <c r="B27" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
-        <v>43637</v>
+        <v>43641</v>
+      </c>
+      <c r="B28" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
-        <v>43640</v>
+        <v>43642</v>
+      </c>
+      <c r="B29" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
-        <v>43641</v>
+        <v>43643</v>
+      </c>
+      <c r="B30" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
-        <v>43642</v>
+        <v>43644</v>
+      </c>
+      <c r="B31" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
-        <v>43643</v>
+        <v>43647</v>
       </c>
       <c r="B32" t="s">
-        <v>5</v>
+        <v>30</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
-        <v>43644</v>
+        <v>43648</v>
+      </c>
+      <c r="B33" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
-        <v>43647</v>
+        <v>43649</v>
       </c>
       <c r="B34" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
-        <v>43648</v>
+        <v>43650</v>
       </c>
       <c r="B35" t="s">
-        <v>2</v>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" s="1">
+        <v>43651</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" s="1">
+        <v>43652</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" s="1">
+        <v>43653</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" s="1">
+        <v>43654</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" s="1">
+        <v>43655</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" s="1">
+        <v>43656</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" s="1">
+        <v>43657</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" s="1">
+        <v>43658</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" s="1">
+        <v>43659</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" s="1">
+        <v>43660</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" s="1">
+        <v>43661</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" s="1">
+        <v>43662</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" s="1">
+        <v>43663</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A49" s="1">
+        <v>43664</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A50" s="1">
+        <v>43665</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A51" s="1">
+        <v>43666</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A52" s="1">
+        <v>43667</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A53" s="1">
+        <v>43668</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A54" s="1">
+        <v>43669</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A55" s="1">
+        <v>43670</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A56" s="1">
+        <v>43671</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A57" s="1">
+        <v>43672</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A58" s="1">
+        <v>43673</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A59" s="1">
+        <v>43674</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A60" s="1">
+        <v>43675</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A61" s="1">
+        <v>43676</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A62" s="1">
+        <v>43677</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A63" s="1">
+        <v>43678</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A64" s="1">
+        <v>43679</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A65" s="1">
+        <v>43680</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A66" s="1">
+        <v>43681</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A67" s="1">
+        <v>43682</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A68" s="1">
+        <v>43683</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A69" s="1">
+        <v>43684</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A70" s="1">
+        <v>43685</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A71" s="1">
+        <v>43686</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A72" s="1">
+        <v>43687</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A73" s="1">
+        <v>43688</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A74" s="1">
+        <v>43689</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Cleaning GitHub to make public
</commit_message>
<xml_diff>
--- a/Workbook.xlsx
+++ b/Workbook.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C23D0AA1-8997-412B-91AD-129C5871E39B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0BE6BCC-7D3C-441B-8AFD-BA3B5DA3438C}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-14910" windowWidth="16440" windowHeight="28440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="54">
   <si>
     <t>Date</t>
   </si>
@@ -170,6 +170,18 @@
   </si>
   <si>
     <t>Working on presentation for feedback session, testing of verified users generator code</t>
+  </si>
+  <si>
+    <t>Trains off, worked from uni on writing disseration - primarily doing captioning</t>
+  </si>
+  <si>
+    <t>Writing dissertation - first half of Network analyiser section done</t>
+  </si>
+  <si>
+    <t>Writing dissertation - second half of Network analyiser and most of topic modeller done</t>
+  </si>
+  <si>
+    <t>Supervision with Gabrila and then worked from the uni</t>
   </si>
 </sst>
 </file>
@@ -503,7 +515,7 @@
   <dimension ref="A1:B89"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="B47" sqref="B47"/>
+      <selection activeCell="B57" sqref="B57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -955,28 +967,40 @@
       <c r="A56" s="2">
         <v>43679</v>
       </c>
+      <c r="B56" s="3" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
         <v>43682</v>
       </c>
+      <c r="B57" s="4" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
         <v>43683</v>
       </c>
       <c r="B58" t="s">
-        <v>4</v>
+        <v>51</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
         <v>43684</v>
       </c>
+      <c r="B59" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
         <v>43685</v>
+      </c>
+      <c r="B60" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="61" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.25">

</xml_diff>